<commit_message>
new black white list
</commit_message>
<xml_diff>
--- a/白名单.xlsx
+++ b/白名单.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>黔源电力</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,6 +118,24 @@
     <t>1. 网传前段时间360借壳概念
 2. 每股营收为负
 3. 前期高点有巨额出货，短期观察为主</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>永清环保</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300187</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.环保行业，算是朝阳行业</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.近期几个明显的大成交量都判断为出货
+2.最近一次运行地位在-20%位置，以观察为主
+3.PE和PB偏高</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +605,7 @@
   <dimension ref="A1:H267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -706,8 +724,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42680</v>
+      </c>
+      <c r="D6" s="1">
+        <v>87.69</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="G6" s="12"/>
+      <c r="H6" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="G7" s="12"/>

</xml_diff>